<commit_message>
Shadow changes and cleaned up settings
</commit_message>
<xml_diff>
--- a/acharyan_captions.xlsx
+++ b/acharyan_captions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="110" windowWidth="34500" windowHeight="16340" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="500" windowWidth="37540" windowHeight="21880"/>
   </bookViews>
   <sheets>
     <sheet name="acharyan_captions" sheetId="3" r:id="rId1"/>
@@ -80,57 +80,24 @@
     <t>Sri Vedānta Lakṣmaṇa Brahmatantra Svatantra Swami (1663 – 1673)</t>
   </si>
   <si>
-    <t>Sri Varada Vedānta Yogīndra Brahmatantra Svatantra Swami (1673 – 1677)</t>
-  </si>
-  <si>
-    <t>Sri Periya Parakāla Brahmatantra Svatantra Mahā Desikan Swami (1677 – 1738)</t>
-  </si>
-  <si>
-    <t>Sri Srinivāsa Brahmatantra Svatantra Swami (1738 – 1751)</t>
-  </si>
-  <si>
-    <t>Sri Vedānta Brahmatantra Svatantra Swami (1751 – 1770)</t>
-  </si>
-  <si>
-    <t>Sri Abhinava Srinivāsa Brahmatantra Svatantra Swami (1770 – 1772)</t>
-  </si>
-  <si>
-    <t>Sri Rāmānuja Brahmatantra Svatantra Swami (1772 – 1810)</t>
-  </si>
-  <si>
-    <t>Sri Ghantāvatāra Brahmatantra Svatantra Swami (1810 – 1827)</t>
-  </si>
-  <si>
-    <t>Sri Vedānta Brahmatantra Svatantra Mahā Desikan Swami (1827 – 1836)</t>
-  </si>
-  <si>
     <t>Sri Srinivāsa Brahmatantra Svatantra Swami (1836 – 1861)</t>
   </si>
   <si>
     <t>Sri Srinivāsa Deśikendra Brahmatantra Svatantra Swami (1861 – 1873)</t>
   </si>
   <si>
-    <t>Sri Raṅganātha Brahmatantra Svatantra Swami (1873 – 1885)</t>
-  </si>
-  <si>
-    <t>Sri Kṛṣṇa Brahmatantra Svatantra Swami (1885 – 1914)</t>
-  </si>
-  <si>
     <t>Sri Vāgīśa Brahmatantra Svatantra Swami (1914 – 1925)</t>
   </si>
   <si>
-    <t>Sri Abhinava Srinivāsa Brahmatantra Svatantra Swami (1967 – 1972)</t>
-  </si>
-  <si>
-    <t>Sri Abhinava Rāmānuja Brahmatantra Svatantra Swami (1972 – 1992)</t>
-  </si>
-  <si>
     <t>Sri Abhinava Vāgīśa Brahmatantra Svatantra Swami (1992 – present)</t>
   </si>
   <si>
     <t>Sri Abhinava Raṅganātha Brahmatantra Svatantra Swami (1925 – 1967)</t>
   </si>
   <si>
+    <t xml:space="preserve"> Sri Vishvaksena</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Swamy Nammāḷvār</t>
   </si>
   <si>
@@ -179,17 +146,50 @@
     <t xml:space="preserve"> Sri Kumāra Varadāchārya</t>
   </si>
   <si>
+    <t>Sri Varada Vedānta Yogīndra Brahmatantra Svatantra Swami (1673 – 1676)</t>
+  </si>
+  <si>
+    <t>Sri Periya Parakāla Brahmatantra Svatantra Mahā Desikan Swami (1676 – 1737)</t>
+  </si>
+  <si>
+    <t>Sri Vedānta Brahmatantra Svatantra Swami (1750 – 1770)</t>
+  </si>
+  <si>
+    <t>Sri Srinivāsa Brahmatantra Svatantra Swami (1738 – 1750)</t>
+  </si>
+  <si>
+    <t>Sri Abhinava Srinivāsa Brahmatantra Svatantra Swami (1770 – 1771)</t>
+  </si>
+  <si>
+    <t>Sri Rāmānuja Brahmatantra Svatantra Swami (1771 – 1811)</t>
+  </si>
+  <si>
+    <t>Sri Ghantāvatāra Brahmatantra Svatantra Swami (1811 – 1829)</t>
+  </si>
+  <si>
+    <t>Sri Vedānta Brahmatantra Svatantra Mahā Desikan Swami (1829 – 1836)</t>
+  </si>
+  <si>
+    <t>Sri Raṅganātha Brahmatantra Svatantra Swami (1873 – 1886)</t>
+  </si>
+  <si>
+    <t>Sri Kṛṣṇa Brahmatantra Svatantra Swami (1886 – 1914)</t>
+  </si>
+  <si>
+    <t>Sri Abhinava Srinivāsa Brahmatantra Svatantra Swami (1967 – 1970)</t>
+  </si>
+  <si>
+    <t>Sri Abhinava Rāmānuja Brahmatantra Svatantra Swami (1971 – 1992)</t>
+  </si>
+  <si>
     <t>Sri Lakshmi Hayagriva</t>
-  </si>
-  <si>
-    <t>Sri Vishvaksena</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -325,8 +325,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -504,6 +511,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -667,14 +680,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -728,6 +740,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1022,373 +1037,376 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.7265625" customWidth="1"/>
-    <col min="2" max="2" width="67.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6328125" customWidth="1"/>
+    <col min="2" max="2" width="89.1796875" customWidth="1"/>
+    <col min="3" max="3" width="23.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B1" t="s">
+    <row r="1" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B21" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B22" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B23" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B24" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B25" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B26" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B27" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>27</v>
       </c>
-      <c r="B28" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B28" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>28</v>
       </c>
-      <c r="B29" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B29" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B30" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>30</v>
       </c>
-      <c r="B31" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B31" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <v>31</v>
       </c>
-      <c r="B32" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B32" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
         <v>32</v>
       </c>
-      <c r="B33" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B33" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
         <v>33</v>
       </c>
-      <c r="B34" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B34" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
         <v>34</v>
       </c>
-      <c r="B35" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B35" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A36" s="1">
         <v>35</v>
       </c>
-      <c r="B36" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B36" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A37" s="1">
         <v>36</v>
       </c>
-      <c r="B37" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B37" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B38" s="2"/>
+    </row>
+    <row r="39" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B39" s="2"/>
+    </row>
+    <row r="40" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A51" s="1"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A54" s="1"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A55" s="1"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A56" s="1"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A57" s="1"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A59" s="1"/>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.35">
@@ -1442,14 +1460,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="2"/>
-    <col min="2" max="2" width="40.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.81640625" style="4"/>
+    <col min="2" max="2" width="40.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -1458,197 +1476,165 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="2">
+      <c r="A2" s="4">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="2">
+      <c r="A4" s="4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="4">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="4">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="4">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="4">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="4">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="4">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="4">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="4">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="4">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="2">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="4">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="3">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="4">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="2">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="4">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="2">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="4">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="3">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="2">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="2">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="3">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="2">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" s="2">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" s="3">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" s="2">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="2">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="3">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="2">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="3"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" s="3"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" s="3"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" s="3"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" s="3"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" s="3"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" s="3"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" s="3"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" s="3"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" s="3"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" s="3"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" s="3"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" s="3"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" s="3"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A34" s="3"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A35" s="3"/>
-    </row>
+    <row r="20" spans="1:2" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:2" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:2" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:2" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:2" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:2" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:2" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:2" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:2" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:2" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:2" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:2" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:2" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="34" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="35" ht="15" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sortState ref="A1:B33">
     <sortCondition ref="A1"/>

</xml_diff>

<commit_message>
From GPT5, new arrangement
</commit_message>
<xml_diff>
--- a/acharyan_captions.xlsx
+++ b/acharyan_captions.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
   <si>
     <t>Founders and Early Āchāryas</t>
   </si>
@@ -183,6 +183,18 @@
   </si>
   <si>
     <t>Sri Lakshmi Hayagriva</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>SL NO</t>
+  </si>
+  <si>
+    <t>CONTEMP</t>
+  </si>
+  <si>
+    <t>IS MAIN</t>
   </si>
 </sst>
 </file>
@@ -1035,10 +1047,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B72"/>
+  <dimension ref="A1:D72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="C2" sqref="C2:C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1048,365 +1060,482 @@
     <col min="3" max="3" width="23.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>57</v>
+      </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C34">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A36" s="1">
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C36">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A37" s="1">
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
     </row>
-    <row r="39" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
     </row>
-    <row r="40" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
     </row>
-    <row r="41" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
     </row>
-    <row r="42" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
     </row>
-    <row r="43" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
     </row>
-    <row r="44" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
     </row>
-    <row r="45" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
     </row>
-    <row r="46" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="1"/>
     </row>
-    <row r="47" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="1"/>
     </row>
-    <row r="48" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="1"/>
     </row>
-    <row r="49" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" s="1"/>
     </row>
-    <row r="50" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" s="1"/>
     </row>
-    <row r="51" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" s="1"/>
     </row>
-    <row r="52" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A52" s="1"/>
     </row>
-    <row r="53" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A53" s="1"/>
     </row>
-    <row r="54" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A54" s="1"/>
     </row>
-    <row r="55" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A55" s="1"/>
     </row>
-    <row r="56" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A56" s="1"/>
     </row>
-    <row r="57" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A57" s="1"/>
     </row>
-    <row r="58" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A58" s="1"/>
     </row>
-    <row r="59" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A59" s="1"/>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.35">
@@ -1458,183 +1587,237 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.81640625" style="4"/>
     <col min="2" max="2" width="40.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.81640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>57</v>
+      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="C2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C4" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="C5" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C6" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C7" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="C8" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C9" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C10" s="4">
+        <v>8</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
         <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C11" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C12" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
         <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C13" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+      <c r="C14" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+      <c r="C15" s="4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
         <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C16" s="4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
         <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C17" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
         <v>16</v>
       </c>
       <c r="B18" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C18" s="4">
+        <v>13</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
         <v>17</v>
       </c>
       <c r="B19" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="1:2" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="1:2" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="1:2" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:2" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:2" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:2" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:2" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:2" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:2" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:2" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:2" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:2" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="33" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="34" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="35" ht="15" x14ac:dyDescent="0.2"/>
+      <c r="C19" s="4">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A1:B33">
     <sortCondition ref="A1"/>

</xml_diff>

<commit_message>
FIxed Svatantra to Swatantra - made consistent. Also checking in resulting PDF
</commit_message>
<xml_diff>
--- a/acharyan_captions.xlsx
+++ b/acharyan_captions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CODING\POSTER\Sri_Parakala_Poster_Template_300DPI\parampara_poster_template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CODING\POSTER\Sri_Parakala_Poster_Template_300DPI\Parampara_Poster\parampara_poster_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86625356-9949-4DFB-BA47-642D2AABFC5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F9DAB4-A1C0-42AF-A31F-0F322B050B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9310" yWindow="3350" windowWidth="28800" windowHeight="15370" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7310" yWindow="2480" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="acharyan_captions" sheetId="1" r:id="rId1"/>
@@ -32,111 +32,6 @@
   </si>
   <si>
     <t>Sri Brahmatantra Swatantra Maha Desikan (1359 – 1386)</t>
-  </si>
-  <si>
-    <t>Sri Dviteeya (Vātsya Vedānta Rāmānuja) Brahmatantra Svatantra Mahā Desikan (1386 – 1394)</t>
-  </si>
-  <si>
-    <t>Sri Tṛtīya (Srinivāsa) Brahmatantra Svatantra Mahā Desikan (1394 – 1406)</t>
-  </si>
-  <si>
-    <t>Sri Parakāla Brahmatantra Svatantra Mahā Desikan (1406 – 1424)</t>
-  </si>
-  <si>
-    <t>Sri Vedānta Rāmānuja Brahmatantra Svatantra Mahā Desikan (1424 – 1440)</t>
-  </si>
-  <si>
-    <t>Sri Srinivāsa Brahmatantra Svatantra Mahā Desikan (1440 – 1460)</t>
-  </si>
-  <si>
-    <t>Sri Nārāyaṇa Yogindra Brahmatantra Svatantra Mahā Desikan (1460 – 1482)</t>
-  </si>
-  <si>
-    <t>Sri Raṅgarāja Yogindra Brahmatantra Svatantra Mahā Desikan (1482 – 1498)</t>
-  </si>
-  <si>
-    <t>Sri Chaturtha Brahmatantra Svatantra Mahā Desikan (1498 – 1517)</t>
-  </si>
-  <si>
-    <t>Sri Yatirāja Brahmatantra Svatantra Mahā Desikan (1517 – 1535)</t>
-  </si>
-  <si>
-    <t>Sri Varada Brahmatantra Svatantra Mahā Desikan (1535 – 1552)</t>
-  </si>
-  <si>
-    <t>Sri Parāṅkuśa Brahmatantra Svatantra Mahā Desikan (1552 – 1567)</t>
-  </si>
-  <si>
-    <t>Sri Kavitārkika Siṃha Brahmatantra Svatantra Mahā Desikan (1567 – 1583)</t>
-  </si>
-  <si>
-    <t>Sri Vedānta Yathivarya Brahmatantra Svatantra Mahā Desikan (1583 – 1607)</t>
-  </si>
-  <si>
-    <t>Sri Jñānābdi Brahmatantra Svatantra Mahā Desikan (1607 – 1618)</t>
-  </si>
-  <si>
-    <t>Sri Vīrarāghava Yogindra Brahmatantra Svatantra Mahā Desikan (1618 – 1640)</t>
-  </si>
-  <si>
-    <t>Sri Varada Vedānta Brahmatantra Svatantra Mahā Desikan (1640 – 1652)</t>
-  </si>
-  <si>
-    <t>Sri Varāha Brahmatantra Svatantra Mahā Desikan (1652 – 1663)</t>
-  </si>
-  <si>
-    <t>Sri Vedānta Lakṣmaṇa Brahmatantra Svatantra Mahā Desikan (1663 – 1673)</t>
-  </si>
-  <si>
-    <t>Sri Varada Vedānta Yogīndra Brahmatantra Svatantra Mahā Desikan (1673 – 1677)</t>
-  </si>
-  <si>
-    <t>Sri Maha Parakāla Brahmatantra Svatantra Mahā Desikan (1676 – 1738)</t>
-  </si>
-  <si>
-    <t>Sri Srinivāsa Brahmatantra Svatantra Parakāla Mahā Desikan (1738 – 1751)</t>
-  </si>
-  <si>
-    <t>Sri Vedānta Brahmatantra Svatantra Parakāla Mahā Desikan (1750 – 1770)</t>
-  </si>
-  <si>
-    <t>Srimat Abhinava Srinivāsa Brahmatantra Svatantra Parakāla Mahā Desikan (1770 – 1772)</t>
-  </si>
-  <si>
-    <t>Sri Rāmānuja Brahmatantra Svatantra Mahā Parakāla Desikan (1772 – 1810)</t>
-  </si>
-  <si>
-    <t>Sri Ghantāvatāra Brahmatantra Svatantra Parakāla Mahā Desikan (1810 – 1829)</t>
-  </si>
-  <si>
-    <t>Sri Vedānta Brahmatantra Svatantra Parakāla Mahā Desikan (1829 – 1836)</t>
-  </si>
-  <si>
-    <t>Sri Srinivāsa Brahmatantra Svatantra Parakāla Mahā Desikan (1836 – 1861)</t>
-  </si>
-  <si>
-    <t>Sri Srinivāsa Deśikendra Brahmatantra Svatantra Parakāla Mahā Desikan (1861 – 1873)</t>
-  </si>
-  <si>
-    <t>Sri Raṅganātha Brahmatantra Svatantra Parakāla Mahā Desikan (1873 – 1885)</t>
-  </si>
-  <si>
-    <t>Sri Kṛṣṇa Brahmatantra Svatantra Parakāla Mahā Desikan (1885 – 1915)</t>
-  </si>
-  <si>
-    <t>Sri Vāgīśa Brahmatantra Svatantra Parakāla Mahā Desikan (1915 – 1925)</t>
-  </si>
-  <si>
-    <t>Srimat Abhinava Raṅganātha Brahmatantra Svatantra Parakāla Mahā Desikan (1925 – 1967)</t>
-  </si>
-  <si>
-    <t>Srimat Abhinava Srinivāsa Brahmatantra Svatantra Parakāla Mahā Desikan (1967 – 1972)</t>
-  </si>
-  <si>
-    <t>Srimat Abhinava Rāmānuja Brahmatantra Svatantra Parakāla Mahā Desikan (1972 – 1992)</t>
-  </si>
-  <si>
-    <t>Srimat Abhinava Vāgīśa Brahmatantra Svatantra Parakāla Mahā Desikan (1992 – present)</t>
   </si>
   <si>
     <t>SL NO</t>
@@ -206,6 +101,111 @@
   </si>
   <si>
     <t>Kidambi Raṅgarājāchārya</t>
+  </si>
+  <si>
+    <t>Sri Dviteeya (Vātsya Vedānta Rāmānuja) Brahmatantra Swatantra Mahā Desikan (1386 – 1394)</t>
+  </si>
+  <si>
+    <t>Sri Tṛtīya (Srinivāsa) Brahmatantra Swatantra Mahā Desikan (1394 – 1406)</t>
+  </si>
+  <si>
+    <t>Sri Parakāla Brahmatantra Swatantra Mahā Desikan (1406 – 1424)</t>
+  </si>
+  <si>
+    <t>Sri Vedānta Rāmānuja Brahmatantra Swatantra Mahā Desikan (1424 – 1440)</t>
+  </si>
+  <si>
+    <t>Sri Srinivāsa Brahmatantra Swatantra Mahā Desikan (1440 – 1460)</t>
+  </si>
+  <si>
+    <t>Sri Nārāyaṇa Yogindra Brahmatantra Swatantra Mahā Desikan (1460 – 1482)</t>
+  </si>
+  <si>
+    <t>Sri Raṅgarāja Yogindra Brahmatantra Swatantra Mahā Desikan (1482 – 1498)</t>
+  </si>
+  <si>
+    <t>Sri Chaturtha Brahmatantra Swatantra Mahā Desikan (1498 – 1517)</t>
+  </si>
+  <si>
+    <t>Sri Yatirāja Brahmatantra Swatantra Mahā Desikan (1517 – 1535)</t>
+  </si>
+  <si>
+    <t>Sri Varada Brahmatantra Swatantra Mahā Desikan (1535 – 1552)</t>
+  </si>
+  <si>
+    <t>Sri Parāṅkuśa Brahmatantra Swatantra Mahā Desikan (1552 – 1567)</t>
+  </si>
+  <si>
+    <t>Sri Kavitārkika Siṃha Brahmatantra Swatantra Mahā Desikan (1567 – 1583)</t>
+  </si>
+  <si>
+    <t>Sri Vedānta Yathivarya Brahmatantra Swatantra Mahā Desikan (1583 – 1607)</t>
+  </si>
+  <si>
+    <t>Sri Jñānābdi Brahmatantra Swatantra Mahā Desikan (1607 – 1618)</t>
+  </si>
+  <si>
+    <t>Sri Vīrarāghava Yogindra Brahmatantra Swatantra Mahā Desikan (1618 – 1640)</t>
+  </si>
+  <si>
+    <t>Sri Varada Vedānta Brahmatantra Swatantra Mahā Desikan (1640 – 1652)</t>
+  </si>
+  <si>
+    <t>Sri Varāha Brahmatantra Swatantra Mahā Desikan (1652 – 1663)</t>
+  </si>
+  <si>
+    <t>Sri Vedānta Lakṣmaṇa Brahmatantra Swatantra Mahā Desikan (1663 – 1673)</t>
+  </si>
+  <si>
+    <t>Sri Varada Vedānta Yogīndra Brahmatantra Swatantra Mahā Desikan (1673 – 1677)</t>
+  </si>
+  <si>
+    <t>Sri Maha Parakāla Brahmatantra Swatantra Mahā Desikan (1676 – 1738)</t>
+  </si>
+  <si>
+    <t>Sri Srinivāsa Brahmatantra Swatantra Parakāla Mahā Desikan (1738 – 1751)</t>
+  </si>
+  <si>
+    <t>Sri Vedānta Brahmatantra Swatantra Parakāla Mahā Desikan (1750 – 1770)</t>
+  </si>
+  <si>
+    <t>Srimat Abhinava Srinivāsa Brahmatantra Swatantra Parakāla Mahā Desikan (1770 – 1772)</t>
+  </si>
+  <si>
+    <t>Sri Rāmānuja Brahmatantra Swatantra Mahā Parakāla Desikan (1772 – 1810)</t>
+  </si>
+  <si>
+    <t>Sri Ghantāvatāra Brahmatantra Swatantra Parakāla Mahā Desikan (1810 – 1829)</t>
+  </si>
+  <si>
+    <t>Sri Vedānta Brahmatantra Swatantra Parakāla Mahā Desikan (1829 – 1836)</t>
+  </si>
+  <si>
+    <t>Sri Srinivāsa Brahmatantra Swatantra Parakāla Mahā Desikan (1836 – 1861)</t>
+  </si>
+  <si>
+    <t>Sri Srinivāsa Deśikendra Brahmatantra Swatantra Parakāla Mahā Desikan (1861 – 1873)</t>
+  </si>
+  <si>
+    <t>Sri Raṅganātha Brahmatantra Swatantra Parakāla Mahā Desikan (1873 – 1885)</t>
+  </si>
+  <si>
+    <t>Sri Kṛṣṇa Brahmatantra Swatantra Parakāla Mahā Desikan (1885 – 1915)</t>
+  </si>
+  <si>
+    <t>Sri Vāgīśa Brahmatantra Swatantra Parakāla Mahā Desikan (1915 – 1925)</t>
+  </si>
+  <si>
+    <t>Srimat Abhinava Raṅganātha Brahmatantra Swatantra Parakāla Mahā Desikan (1925 – 1967)</t>
+  </si>
+  <si>
+    <t>Srimat Abhinava Srinivāsa Brahmatantra Swatantra Parakāla Mahā Desikan (1967 – 1972)</t>
+  </si>
+  <si>
+    <t>Srimat Abhinava Rāmānuja Brahmatantra Swatantra Parakāla Mahā Desikan (1972 – 1992)</t>
+  </si>
+  <si>
+    <t>Srimat Abhinava Vāgīśa Brahmatantra Swatantra Parakāla Mahā Desikan (1992 – present)</t>
   </si>
 </sst>
 </file>
@@ -364,10 +364,10 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -585,7 +585,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
@@ -662,10 +662,10 @@
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="27" t="s">
-        <v>2</v>
+      <c r="B3" s="28" t="s">
+        <v>25</v>
       </c>
-      <c r="C3" s="26"/>
+      <c r="C3" s="27"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -695,7 +695,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -727,7 +727,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -759,7 +759,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -791,7 +791,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -823,7 +823,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -855,7 +855,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -887,7 +887,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -919,7 +919,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -951,7 +951,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -983,7 +983,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1015,7 +1015,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -1047,7 +1047,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -1079,7 +1079,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -1111,7 +1111,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
@@ -1143,7 +1143,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
@@ -1175,7 +1175,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
@@ -1207,7 +1207,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
@@ -1239,7 +1239,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -1271,7 +1271,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -1303,7 +1303,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -1335,7 +1335,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
@@ -1366,10 +1366,10 @@
       <c r="A25" s="4">
         <v>24</v>
       </c>
-      <c r="B25" s="25" t="s">
-        <v>24</v>
+      <c r="B25" s="26" t="s">
+        <v>47</v>
       </c>
-      <c r="C25" s="26"/>
+      <c r="C25" s="27"/>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
@@ -1399,7 +1399,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -1431,7 +1431,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
@@ -1463,7 +1463,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -1495,7 +1495,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -1526,10 +1526,10 @@
       <c r="A30" s="4">
         <v>29</v>
       </c>
-      <c r="B30" s="25" t="s">
-        <v>29</v>
+      <c r="B30" s="26" t="s">
+        <v>52</v>
       </c>
-      <c r="C30" s="26"/>
+      <c r="C30" s="27"/>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
@@ -1559,7 +1559,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
@@ -1591,7 +1591,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
@@ -1623,7 +1623,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
@@ -1654,10 +1654,10 @@
       <c r="A34" s="4">
         <v>33</v>
       </c>
-      <c r="B34" s="25" t="s">
-        <v>33</v>
+      <c r="B34" s="26" t="s">
+        <v>56</v>
       </c>
-      <c r="C34" s="26"/>
+      <c r="C34" s="27"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
@@ -1686,10 +1686,10 @@
       <c r="A35" s="4">
         <v>34</v>
       </c>
-      <c r="B35" s="25" t="s">
-        <v>34</v>
+      <c r="B35" s="26" t="s">
+        <v>57</v>
       </c>
-      <c r="C35" s="26"/>
+      <c r="C35" s="27"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
@@ -1718,10 +1718,10 @@
       <c r="A36" s="4">
         <v>35</v>
       </c>
-      <c r="B36" s="25" t="s">
-        <v>35</v>
+      <c r="B36" s="26" t="s">
+        <v>58</v>
       </c>
-      <c r="C36" s="26"/>
+      <c r="C36" s="27"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
@@ -1750,10 +1750,10 @@
       <c r="A37" s="4">
         <v>36</v>
       </c>
-      <c r="B37" s="25" t="s">
-        <v>36</v>
+      <c r="B37" s="26" t="s">
+        <v>59</v>
       </c>
-      <c r="C37" s="26"/>
+      <c r="C37" s="27"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
@@ -28761,7 +28761,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0139F442-1B47-40FE-BE5B-EBE8D8F2F5C2}">
   <dimension ref="A1:L999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
@@ -28777,16 +28777,16 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>37</v>
+        <v>2</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
@@ -28794,7 +28794,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="D2" s="20">
         <v>0</v>
@@ -28805,7 +28805,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="D3" s="19">
         <v>1</v>
@@ -28817,7 +28817,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="D4" s="20">
         <v>2</v>
@@ -28829,7 +28829,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="D5" s="21">
         <v>3</v>
@@ -28841,7 +28841,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="D6" s="19">
         <v>4</v>
@@ -28853,7 +28853,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="D7" s="20">
         <v>5</v>
@@ -28865,7 +28865,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="D8" s="21">
         <v>6</v>
@@ -28877,7 +28877,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="D9" s="19">
         <v>7</v>
@@ -28889,13 +28889,13 @@
         <v>8</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="D10" s="20">
         <v>8</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="K10" s="15"/>
     </row>
@@ -28904,7 +28904,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="D11" s="20">
         <v>9</v>
@@ -28916,7 +28916,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>46</v>
+        <v>11</v>
       </c>
       <c r="D12" s="20">
         <v>9</v>
@@ -28927,8 +28927,8 @@
       <c r="A13" s="11">
         <v>11</v>
       </c>
-      <c r="C13" s="28" t="s">
-        <v>58</v>
+      <c r="C13" s="25" t="s">
+        <v>23</v>
       </c>
       <c r="D13" s="20">
         <v>10</v>
@@ -28941,7 +28941,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="D14" s="20">
         <v>10</v>
@@ -28954,7 +28954,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="D15" s="20">
         <v>11</v>
@@ -28967,7 +28967,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="D16" s="20">
         <v>11</v>
@@ -28978,7 +28978,7 @@
         <v>15</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="D17" s="22">
         <v>12</v>
@@ -28989,13 +28989,13 @@
         <v>16</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="D18" s="22">
         <v>13</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -29003,7 +29003,7 @@
         <v>17</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="D19" s="23">
         <v>14</v>

</xml_diff>

<commit_message>
HTML with latest data
</commit_message>
<xml_diff>
--- a/acharyan_captions.xlsx
+++ b/acharyan_captions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CODING\POSTER\Sri_Parakala_Poster_Template_300DPI\parampara_poster_template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CODING\POSTER\Sri_Parakala_Poster_Template_300DPI\Parampara_Poster\parampara_poster_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86625356-9949-4DFB-BA47-642D2AABFC5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F9DAB4-A1C0-42AF-A31F-0F322B050B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9310" yWindow="3350" windowWidth="28800" windowHeight="15370" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7310" yWindow="2480" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="acharyan_captions" sheetId="1" r:id="rId1"/>
@@ -32,111 +32,6 @@
   </si>
   <si>
     <t>Sri Brahmatantra Swatantra Maha Desikan (1359 – 1386)</t>
-  </si>
-  <si>
-    <t>Sri Dviteeya (Vātsya Vedānta Rāmānuja) Brahmatantra Svatantra Mahā Desikan (1386 – 1394)</t>
-  </si>
-  <si>
-    <t>Sri Tṛtīya (Srinivāsa) Brahmatantra Svatantra Mahā Desikan (1394 – 1406)</t>
-  </si>
-  <si>
-    <t>Sri Parakāla Brahmatantra Svatantra Mahā Desikan (1406 – 1424)</t>
-  </si>
-  <si>
-    <t>Sri Vedānta Rāmānuja Brahmatantra Svatantra Mahā Desikan (1424 – 1440)</t>
-  </si>
-  <si>
-    <t>Sri Srinivāsa Brahmatantra Svatantra Mahā Desikan (1440 – 1460)</t>
-  </si>
-  <si>
-    <t>Sri Nārāyaṇa Yogindra Brahmatantra Svatantra Mahā Desikan (1460 – 1482)</t>
-  </si>
-  <si>
-    <t>Sri Raṅgarāja Yogindra Brahmatantra Svatantra Mahā Desikan (1482 – 1498)</t>
-  </si>
-  <si>
-    <t>Sri Chaturtha Brahmatantra Svatantra Mahā Desikan (1498 – 1517)</t>
-  </si>
-  <si>
-    <t>Sri Yatirāja Brahmatantra Svatantra Mahā Desikan (1517 – 1535)</t>
-  </si>
-  <si>
-    <t>Sri Varada Brahmatantra Svatantra Mahā Desikan (1535 – 1552)</t>
-  </si>
-  <si>
-    <t>Sri Parāṅkuśa Brahmatantra Svatantra Mahā Desikan (1552 – 1567)</t>
-  </si>
-  <si>
-    <t>Sri Kavitārkika Siṃha Brahmatantra Svatantra Mahā Desikan (1567 – 1583)</t>
-  </si>
-  <si>
-    <t>Sri Vedānta Yathivarya Brahmatantra Svatantra Mahā Desikan (1583 – 1607)</t>
-  </si>
-  <si>
-    <t>Sri Jñānābdi Brahmatantra Svatantra Mahā Desikan (1607 – 1618)</t>
-  </si>
-  <si>
-    <t>Sri Vīrarāghava Yogindra Brahmatantra Svatantra Mahā Desikan (1618 – 1640)</t>
-  </si>
-  <si>
-    <t>Sri Varada Vedānta Brahmatantra Svatantra Mahā Desikan (1640 – 1652)</t>
-  </si>
-  <si>
-    <t>Sri Varāha Brahmatantra Svatantra Mahā Desikan (1652 – 1663)</t>
-  </si>
-  <si>
-    <t>Sri Vedānta Lakṣmaṇa Brahmatantra Svatantra Mahā Desikan (1663 – 1673)</t>
-  </si>
-  <si>
-    <t>Sri Varada Vedānta Yogīndra Brahmatantra Svatantra Mahā Desikan (1673 – 1677)</t>
-  </si>
-  <si>
-    <t>Sri Maha Parakāla Brahmatantra Svatantra Mahā Desikan (1676 – 1738)</t>
-  </si>
-  <si>
-    <t>Sri Srinivāsa Brahmatantra Svatantra Parakāla Mahā Desikan (1738 – 1751)</t>
-  </si>
-  <si>
-    <t>Sri Vedānta Brahmatantra Svatantra Parakāla Mahā Desikan (1750 – 1770)</t>
-  </si>
-  <si>
-    <t>Srimat Abhinava Srinivāsa Brahmatantra Svatantra Parakāla Mahā Desikan (1770 – 1772)</t>
-  </si>
-  <si>
-    <t>Sri Rāmānuja Brahmatantra Svatantra Mahā Parakāla Desikan (1772 – 1810)</t>
-  </si>
-  <si>
-    <t>Sri Ghantāvatāra Brahmatantra Svatantra Parakāla Mahā Desikan (1810 – 1829)</t>
-  </si>
-  <si>
-    <t>Sri Vedānta Brahmatantra Svatantra Parakāla Mahā Desikan (1829 – 1836)</t>
-  </si>
-  <si>
-    <t>Sri Srinivāsa Brahmatantra Svatantra Parakāla Mahā Desikan (1836 – 1861)</t>
-  </si>
-  <si>
-    <t>Sri Srinivāsa Deśikendra Brahmatantra Svatantra Parakāla Mahā Desikan (1861 – 1873)</t>
-  </si>
-  <si>
-    <t>Sri Raṅganātha Brahmatantra Svatantra Parakāla Mahā Desikan (1873 – 1885)</t>
-  </si>
-  <si>
-    <t>Sri Kṛṣṇa Brahmatantra Svatantra Parakāla Mahā Desikan (1885 – 1915)</t>
-  </si>
-  <si>
-    <t>Sri Vāgīśa Brahmatantra Svatantra Parakāla Mahā Desikan (1915 – 1925)</t>
-  </si>
-  <si>
-    <t>Srimat Abhinava Raṅganātha Brahmatantra Svatantra Parakāla Mahā Desikan (1925 – 1967)</t>
-  </si>
-  <si>
-    <t>Srimat Abhinava Srinivāsa Brahmatantra Svatantra Parakāla Mahā Desikan (1967 – 1972)</t>
-  </si>
-  <si>
-    <t>Srimat Abhinava Rāmānuja Brahmatantra Svatantra Parakāla Mahā Desikan (1972 – 1992)</t>
-  </si>
-  <si>
-    <t>Srimat Abhinava Vāgīśa Brahmatantra Svatantra Parakāla Mahā Desikan (1992 – present)</t>
   </si>
   <si>
     <t>SL NO</t>
@@ -206,6 +101,111 @@
   </si>
   <si>
     <t>Kidambi Raṅgarājāchārya</t>
+  </si>
+  <si>
+    <t>Sri Dviteeya (Vātsya Vedānta Rāmānuja) Brahmatantra Swatantra Mahā Desikan (1386 – 1394)</t>
+  </si>
+  <si>
+    <t>Sri Tṛtīya (Srinivāsa) Brahmatantra Swatantra Mahā Desikan (1394 – 1406)</t>
+  </si>
+  <si>
+    <t>Sri Parakāla Brahmatantra Swatantra Mahā Desikan (1406 – 1424)</t>
+  </si>
+  <si>
+    <t>Sri Vedānta Rāmānuja Brahmatantra Swatantra Mahā Desikan (1424 – 1440)</t>
+  </si>
+  <si>
+    <t>Sri Srinivāsa Brahmatantra Swatantra Mahā Desikan (1440 – 1460)</t>
+  </si>
+  <si>
+    <t>Sri Nārāyaṇa Yogindra Brahmatantra Swatantra Mahā Desikan (1460 – 1482)</t>
+  </si>
+  <si>
+    <t>Sri Raṅgarāja Yogindra Brahmatantra Swatantra Mahā Desikan (1482 – 1498)</t>
+  </si>
+  <si>
+    <t>Sri Chaturtha Brahmatantra Swatantra Mahā Desikan (1498 – 1517)</t>
+  </si>
+  <si>
+    <t>Sri Yatirāja Brahmatantra Swatantra Mahā Desikan (1517 – 1535)</t>
+  </si>
+  <si>
+    <t>Sri Varada Brahmatantra Swatantra Mahā Desikan (1535 – 1552)</t>
+  </si>
+  <si>
+    <t>Sri Parāṅkuśa Brahmatantra Swatantra Mahā Desikan (1552 – 1567)</t>
+  </si>
+  <si>
+    <t>Sri Kavitārkika Siṃha Brahmatantra Swatantra Mahā Desikan (1567 – 1583)</t>
+  </si>
+  <si>
+    <t>Sri Vedānta Yathivarya Brahmatantra Swatantra Mahā Desikan (1583 – 1607)</t>
+  </si>
+  <si>
+    <t>Sri Jñānābdi Brahmatantra Swatantra Mahā Desikan (1607 – 1618)</t>
+  </si>
+  <si>
+    <t>Sri Vīrarāghava Yogindra Brahmatantra Swatantra Mahā Desikan (1618 – 1640)</t>
+  </si>
+  <si>
+    <t>Sri Varada Vedānta Brahmatantra Swatantra Mahā Desikan (1640 – 1652)</t>
+  </si>
+  <si>
+    <t>Sri Varāha Brahmatantra Swatantra Mahā Desikan (1652 – 1663)</t>
+  </si>
+  <si>
+    <t>Sri Vedānta Lakṣmaṇa Brahmatantra Swatantra Mahā Desikan (1663 – 1673)</t>
+  </si>
+  <si>
+    <t>Sri Varada Vedānta Yogīndra Brahmatantra Swatantra Mahā Desikan (1673 – 1677)</t>
+  </si>
+  <si>
+    <t>Sri Maha Parakāla Brahmatantra Swatantra Mahā Desikan (1676 – 1738)</t>
+  </si>
+  <si>
+    <t>Sri Srinivāsa Brahmatantra Swatantra Parakāla Mahā Desikan (1738 – 1751)</t>
+  </si>
+  <si>
+    <t>Sri Vedānta Brahmatantra Swatantra Parakāla Mahā Desikan (1750 – 1770)</t>
+  </si>
+  <si>
+    <t>Srimat Abhinava Srinivāsa Brahmatantra Swatantra Parakāla Mahā Desikan (1770 – 1772)</t>
+  </si>
+  <si>
+    <t>Sri Rāmānuja Brahmatantra Swatantra Mahā Parakāla Desikan (1772 – 1810)</t>
+  </si>
+  <si>
+    <t>Sri Ghantāvatāra Brahmatantra Swatantra Parakāla Mahā Desikan (1810 – 1829)</t>
+  </si>
+  <si>
+    <t>Sri Vedānta Brahmatantra Swatantra Parakāla Mahā Desikan (1829 – 1836)</t>
+  </si>
+  <si>
+    <t>Sri Srinivāsa Brahmatantra Swatantra Parakāla Mahā Desikan (1836 – 1861)</t>
+  </si>
+  <si>
+    <t>Sri Srinivāsa Deśikendra Brahmatantra Swatantra Parakāla Mahā Desikan (1861 – 1873)</t>
+  </si>
+  <si>
+    <t>Sri Raṅganātha Brahmatantra Swatantra Parakāla Mahā Desikan (1873 – 1885)</t>
+  </si>
+  <si>
+    <t>Sri Kṛṣṇa Brahmatantra Swatantra Parakāla Mahā Desikan (1885 – 1915)</t>
+  </si>
+  <si>
+    <t>Sri Vāgīśa Brahmatantra Swatantra Parakāla Mahā Desikan (1915 – 1925)</t>
+  </si>
+  <si>
+    <t>Srimat Abhinava Raṅganātha Brahmatantra Swatantra Parakāla Mahā Desikan (1925 – 1967)</t>
+  </si>
+  <si>
+    <t>Srimat Abhinava Srinivāsa Brahmatantra Swatantra Parakāla Mahā Desikan (1967 – 1972)</t>
+  </si>
+  <si>
+    <t>Srimat Abhinava Rāmānuja Brahmatantra Swatantra Parakāla Mahā Desikan (1972 – 1992)</t>
+  </si>
+  <si>
+    <t>Srimat Abhinava Vāgīśa Brahmatantra Swatantra Parakāla Mahā Desikan (1992 – present)</t>
   </si>
 </sst>
 </file>
@@ -364,10 +364,10 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -585,7 +585,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
@@ -662,10 +662,10 @@
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="27" t="s">
-        <v>2</v>
+      <c r="B3" s="28" t="s">
+        <v>25</v>
       </c>
-      <c r="C3" s="26"/>
+      <c r="C3" s="27"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -695,7 +695,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -727,7 +727,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -759,7 +759,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -791,7 +791,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -823,7 +823,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -855,7 +855,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -887,7 +887,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -919,7 +919,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -951,7 +951,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -983,7 +983,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1015,7 +1015,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -1047,7 +1047,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -1079,7 +1079,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -1111,7 +1111,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
@@ -1143,7 +1143,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
@@ -1175,7 +1175,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
@@ -1207,7 +1207,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
@@ -1239,7 +1239,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -1271,7 +1271,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -1303,7 +1303,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -1335,7 +1335,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
@@ -1366,10 +1366,10 @@
       <c r="A25" s="4">
         <v>24</v>
       </c>
-      <c r="B25" s="25" t="s">
-        <v>24</v>
+      <c r="B25" s="26" t="s">
+        <v>47</v>
       </c>
-      <c r="C25" s="26"/>
+      <c r="C25" s="27"/>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
@@ -1399,7 +1399,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -1431,7 +1431,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
@@ -1463,7 +1463,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -1495,7 +1495,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -1526,10 +1526,10 @@
       <c r="A30" s="4">
         <v>29</v>
       </c>
-      <c r="B30" s="25" t="s">
-        <v>29</v>
+      <c r="B30" s="26" t="s">
+        <v>52</v>
       </c>
-      <c r="C30" s="26"/>
+      <c r="C30" s="27"/>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
@@ -1559,7 +1559,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
@@ -1591,7 +1591,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
@@ -1623,7 +1623,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
@@ -1654,10 +1654,10 @@
       <c r="A34" s="4">
         <v>33</v>
       </c>
-      <c r="B34" s="25" t="s">
-        <v>33</v>
+      <c r="B34" s="26" t="s">
+        <v>56</v>
       </c>
-      <c r="C34" s="26"/>
+      <c r="C34" s="27"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
@@ -1686,10 +1686,10 @@
       <c r="A35" s="4">
         <v>34</v>
       </c>
-      <c r="B35" s="25" t="s">
-        <v>34</v>
+      <c r="B35" s="26" t="s">
+        <v>57</v>
       </c>
-      <c r="C35" s="26"/>
+      <c r="C35" s="27"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
@@ -1718,10 +1718,10 @@
       <c r="A36" s="4">
         <v>35</v>
       </c>
-      <c r="B36" s="25" t="s">
-        <v>35</v>
+      <c r="B36" s="26" t="s">
+        <v>58</v>
       </c>
-      <c r="C36" s="26"/>
+      <c r="C36" s="27"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
@@ -1750,10 +1750,10 @@
       <c r="A37" s="4">
         <v>36</v>
       </c>
-      <c r="B37" s="25" t="s">
-        <v>36</v>
+      <c r="B37" s="26" t="s">
+        <v>59</v>
       </c>
-      <c r="C37" s="26"/>
+      <c r="C37" s="27"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
@@ -28761,7 +28761,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0139F442-1B47-40FE-BE5B-EBE8D8F2F5C2}">
   <dimension ref="A1:L999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
@@ -28777,16 +28777,16 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>37</v>
+        <v>2</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
@@ -28794,7 +28794,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="D2" s="20">
         <v>0</v>
@@ -28805,7 +28805,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="D3" s="19">
         <v>1</v>
@@ -28817,7 +28817,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="D4" s="20">
         <v>2</v>
@@ -28829,7 +28829,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="D5" s="21">
         <v>3</v>
@@ -28841,7 +28841,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="D6" s="19">
         <v>4</v>
@@ -28853,7 +28853,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="D7" s="20">
         <v>5</v>
@@ -28865,7 +28865,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="D8" s="21">
         <v>6</v>
@@ -28877,7 +28877,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="D9" s="19">
         <v>7</v>
@@ -28889,13 +28889,13 @@
         <v>8</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="D10" s="20">
         <v>8</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="K10" s="15"/>
     </row>
@@ -28904,7 +28904,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="D11" s="20">
         <v>9</v>
@@ -28916,7 +28916,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>46</v>
+        <v>11</v>
       </c>
       <c r="D12" s="20">
         <v>9</v>
@@ -28927,8 +28927,8 @@
       <c r="A13" s="11">
         <v>11</v>
       </c>
-      <c r="C13" s="28" t="s">
-        <v>58</v>
+      <c r="C13" s="25" t="s">
+        <v>23</v>
       </c>
       <c r="D13" s="20">
         <v>10</v>
@@ -28941,7 +28941,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="D14" s="20">
         <v>10</v>
@@ -28954,7 +28954,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="D15" s="20">
         <v>11</v>
@@ -28967,7 +28967,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="D16" s="20">
         <v>11</v>
@@ -28978,7 +28978,7 @@
         <v>15</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="D17" s="22">
         <v>12</v>
@@ -28989,13 +28989,13 @@
         <v>16</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="D18" s="22">
         <v>13</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -29003,7 +29003,7 @@
         <v>17</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="D19" s="23">
         <v>14</v>

</xml_diff>